<commit_message>
Fixed serializer, glob order lookup
</commit_message>
<xml_diff>
--- a/WorkBot/refactor/data/orders/A.L. George/A.L. George_Collegetown_2025-09-19.xlsx
+++ b/WorkBot/refactor/data/orders/A.L. George/A.L. George_Collegetown_2025-09-19.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>77220</t>
+          <t>77802</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Guayaki Yerba Mate - Enlighten Mint</t>
+          <t>Ithaca Soda - Ginger Beer</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,24 +466,24 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>28.00</t>
+          <t>23.95</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>28.00</t>
+          <t>23.95</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>77802</t>
+          <t>77801</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ithaca Soda - Ginger Beer</t>
+          <t>Ithaca Soda - Root Beer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,39 +505,39 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>77801</t>
+          <t>75112</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ithaca Soda - Root Beer</t>
+          <t>Fiji Water 1L</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>23.95</t>
+          <t>16.50</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>23.95</t>
+          <t>49.50</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>75112</t>
+          <t>77220</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fiji Water 1L</t>
+          <t>Guayaki Yerba Mate - Enlighten Mint</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -547,12 +547,66 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>16.50</t>
+          <t>28.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>33.00</t>
+          <t>56.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>77221</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Guayaki Yerba Mate - Revel Berry</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>28.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>56.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>77222</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Guayaki Yerba Mate - Bluephoria</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>28.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>56.00</t>
         </is>
       </c>
     </row>

</xml_diff>